<commit_message>
Removing the extra sheet
</commit_message>
<xml_diff>
--- a/exercises/Exercise2/DetermineApproversRule.xlsx
+++ b/exercises/Exercise2/DetermineApproversRule.xlsx
@@ -1,17 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22812"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_D71D258B56E04E39A81D9C2B7B170DF3C36199A7" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{17953507-F5B7-4638-86EF-EEB784F2A185}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/i047246/Downloads/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C54BAC91-32E3-8242-A382-56819330C8BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="0" windowHeight="0" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16220" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="DetermineApproversRule" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028" refMode="R1C1" iterateCount="0" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -26,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="38">
   <si>
     <t>Project Name</t>
   </si>
@@ -146,7 +150,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -606,16 +610,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="A7" sqref="A6:G10"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
     <col min="1" max="7" width="40" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="12.75">
+    <row r="1" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -629,7 +633,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A2" s="3" t="s">
         <v>4</v>
       </c>
@@ -643,7 +647,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A3" s="9" t="s">
         <v>8</v>
       </c>
@@ -656,7 +660,7 @@
       <c r="F3" s="9"/>
       <c r="G3" s="9"/>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
@@ -679,7 +683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.15">
       <c r="A5" s="4" t="s">
         <v>17</v>
       </c>
@@ -702,7 +706,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A6" s="5" t="s">
         <v>19</v>
       </c>
@@ -725,7 +729,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A7" s="7" t="s">
         <v>24</v>
       </c>
@@ -746,7 +750,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A8" s="7"/>
       <c r="B8" s="7"/>
       <c r="C8" s="5" t="s">
@@ -765,7 +769,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A9" s="7" t="s">
         <v>30</v>
       </c>
@@ -788,7 +792,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" ht="14" x14ac:dyDescent="0.15">
       <c r="A10" s="8"/>
       <c r="B10" s="6" t="s">
         <v>35</v>
@@ -821,140 +825,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB9FED67-D5DF-4890-AAA0-10BC65A202DD}">
-  <dimension ref="B5:H9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6:B7"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75"/>
-  <sheetData>
-    <row r="5" spans="2:8" ht="25.5">
-      <c r="B5" s="5" t="s">
-        <v>19</v>
-      </c>
-      <c r="C5" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H5" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" ht="25.5">
-      <c r="B6" s="7" t="s">
-        <v>24</v>
-      </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="5" t="s">
-        <v>25</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="H6" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="2:8" ht="25.5">
-      <c r="B7" s="7"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F7" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H7" s="5" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="8" spans="2:8" ht="63.75">
-      <c r="B8" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="D8" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="E8" s="5" t="s">
-        <v>33</v>
-      </c>
-      <c r="F8" s="5" t="s">
-        <v>34</v>
-      </c>
-      <c r="G8" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="H8" s="5" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="9" spans="2:8" ht="25.5">
-      <c r="B9" s="8"/>
-      <c r="C9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="E9" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="G9" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="H9" s="6" t="s">
-        <v>23</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="C5:C7"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101003148741768698445B8941B5ABDBA9457" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="bd83e5515a5bf452121c582ead05a62f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="10c732b3-e810-4ef1-9e4d-ba89bc458783" xmlns:ns3="b94e3b65-f586-4d64-a5a6-c3ffd8dcb7a9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="78fe86c591460e4ec9c36a9f823ca3ee" ns2:_="" ns3:_="">
     <xsd:import namespace="10c732b3-e810-4ef1-9e4d-ba89bc458783"/>
@@ -1165,6 +1036,12 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -1175,13 +1052,37 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDA08B2F-6921-4D2E-A315-B72D0C0EA618}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC00BD0B-8B90-4D61-A580-DDC0842A8261}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="10c732b3-e810-4ef1-9e4d-ba89bc458783"/>
+    <ds:schemaRef ds:uri="b94e3b65-f586-4d64-a5a6-c3ffd8dcb7a9"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{CC00BD0B-8B90-4D61-A580-DDC0842A8261}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{DDA08B2F-6921-4D2E-A315-B72D0C0EA618}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1EE219-9170-4F44-A21E-41076E60C25F}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{BF1EE219-9170-4F44-A21E-41076E60C25F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>